<commit_message>
Adding in new calibration parameters
</commit_message>
<xml_diff>
--- a/projects/office_calibration_rgenoud_14.xlsx
+++ b/projects/office_calibration_rgenoud_14.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$158</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2597" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2614" uniqueCount="828">
   <si>
     <t>type</t>
   </si>
@@ -2320,9 +2320,6 @@
     <t>West Window to Wall Ratio</t>
   </si>
   <si>
-    <t>Space Infiltration Power Reduction</t>
-  </si>
-  <si>
     <t>Lighting Power Reduction</t>
   </si>
   <si>
@@ -2501,6 +2498,33 @@
   </si>
   <si>
     <t>gal</t>
+  </si>
+  <si>
+    <t>Constant Coefficient</t>
+  </si>
+  <si>
+    <t>constant_coefficient</t>
+  </si>
+  <si>
+    <t>temperature_coefficient</t>
+  </si>
+  <si>
+    <t>Temperature Coefficient</t>
+  </si>
+  <si>
+    <t>wind_speed_coefficient</t>
+  </si>
+  <si>
+    <t>Wind Speed Coefficient</t>
+  </si>
+  <si>
+    <t>wind_speed_squared_coefficient</t>
+  </si>
+  <si>
+    <t>Wind Speed Squared Coefficient</t>
+  </si>
+  <si>
+    <t>Space Infiltration Reduction</t>
   </si>
 </sst>
 </file>
@@ -6861,7 +6885,7 @@
         <v>470</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>472</v>
@@ -6932,7 +6956,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6943,7 +6967,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>747</v>
@@ -6954,7 +6978,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>747</v>
@@ -7178,13 +7202,13 @@
     </row>
     <row r="35" spans="1:5" s="31" customFormat="1">
       <c r="A35" s="31" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B35" s="30">
         <v>1</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D35" s="2"/>
     </row>
@@ -7261,7 +7285,7 @@
         <v>699</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1">
@@ -7292,11 +7316,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y227"/>
+  <dimension ref="A1:Y231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N75" sqref="N75"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -7560,7 +7584,7 @@
         <v>618</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -8018,13 +8042,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="38" t="s">
+        <v>772</v>
+      </c>
+      <c r="C33" s="38" t="s">
         <v>773</v>
       </c>
-      <c r="C33" s="38" t="s">
-        <v>774</v>
-      </c>
       <c r="D33" s="38" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>68</v>
@@ -8037,10 +8061,10 @@
         <v>22</v>
       </c>
       <c r="D34" s="43" t="s">
+        <v>761</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>762</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>763</v>
       </c>
       <c r="F34" s="43" t="s">
         <v>64</v>
@@ -8073,10 +8097,10 @@
         <v>22</v>
       </c>
       <c r="D35" s="43" t="s">
+        <v>763</v>
+      </c>
+      <c r="E35" s="43" t="s">
         <v>764</v>
-      </c>
-      <c r="E35" s="43" t="s">
-        <v>765</v>
       </c>
       <c r="F35" s="43" t="s">
         <v>64</v>
@@ -8109,7 +8133,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>74</v>
@@ -8128,7 +8152,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E37" s="43" t="s">
         <v>75</v>
@@ -8137,7 +8161,7 @@
         <v>619</v>
       </c>
       <c r="G37" s="43" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H37" s="43">
         <v>0</v>
@@ -8659,7 +8683,7 @@
         <v>618</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I57" s="31"/>
     </row>
@@ -8677,7 +8701,7 @@
         <v>618</v>
       </c>
       <c r="H58" s="41" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I58" s="31"/>
     </row>
@@ -8686,13 +8710,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="38" t="s">
+        <v>811</v>
+      </c>
+      <c r="C59" s="38" t="s">
         <v>812</v>
       </c>
-      <c r="C59" s="38" t="s">
-        <v>813</v>
-      </c>
       <c r="D59" s="38" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E59" s="38" t="s">
         <v>68</v>
@@ -8705,16 +8729,16 @@
         <v>21</v>
       </c>
       <c r="D60" s="31" t="s">
+        <v>813</v>
+      </c>
+      <c r="E60" s="31" t="s">
         <v>814</v>
-      </c>
-      <c r="E60" s="31" t="s">
-        <v>815</v>
       </c>
       <c r="F60" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H60" s="31" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I60" s="31"/>
     </row>
@@ -8723,16 +8747,16 @@
         <v>22</v>
       </c>
       <c r="D61" s="43" t="s">
+        <v>816</v>
+      </c>
+      <c r="E61" s="43" t="s">
         <v>817</v>
-      </c>
-      <c r="E61" s="43" t="s">
-        <v>818</v>
       </c>
       <c r="F61" s="43" t="s">
         <v>619</v>
       </c>
       <c r="G61" s="43" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H61" s="43">
         <v>1</v>
@@ -9090,7 +9114,7 @@
         <v>22</v>
       </c>
       <c r="D77" s="44" t="s">
-        <v>759</v>
+        <v>827</v>
       </c>
       <c r="E77" s="43" t="s">
         <v>70</v>
@@ -9126,190 +9150,156 @@
         <v>21</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>71</v>
+        <v>819</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>48</v>
+        <v>820</v>
       </c>
       <c r="F78" s="30" t="s">
         <v>64</v>
       </c>
       <c r="H78" s="30">
-        <v>0</v>
-      </c>
-      <c r="O78" s="31"/>
-    </row>
-    <row r="79" spans="1:17" s="30" customFormat="1">
-      <c r="B79" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F79" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" s="43" customFormat="1">
+      <c r="B79" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" s="44" t="s">
+        <v>822</v>
+      </c>
+      <c r="E79" s="43" t="s">
+        <v>821</v>
+      </c>
+      <c r="F79" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H79" s="30">
-        <v>0</v>
-      </c>
-      <c r="O79" s="31"/>
+      <c r="H79" s="43">
+        <v>0</v>
+      </c>
+      <c r="J79" s="45">
+        <v>0</v>
+      </c>
+      <c r="K79" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="L79" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="M79" s="45">
+        <f>(K79-J79)/6</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="N79" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="Q79" s="43" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="80" spans="1:17" s="30" customFormat="1">
       <c r="B80" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D80" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>823</v>
+      </c>
+      <c r="F80" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" s="30" customFormat="1">
+      <c r="B81" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D81" s="30" t="s">
+        <v>826</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>825</v>
+      </c>
+      <c r="F81" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H81" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" s="30" customFormat="1">
+      <c r="B82" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F82" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H82" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" s="30" customFormat="1">
+      <c r="B83" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F83" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H83" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" s="30" customFormat="1">
+      <c r="B84" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D84" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E80" s="30" t="s">
+      <c r="E84" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F80" s="30" t="s">
+      <c r="F84" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="H80" s="30">
+      <c r="H84" s="30">
         <v>1</v>
       </c>
-      <c r="O80" s="31"/>
-    </row>
-    <row r="81" spans="1:17" s="50" customFormat="1">
-      <c r="A81" s="50" t="b">
+      <c r="O84" s="31"/>
+    </row>
+    <row r="85" spans="1:17" s="50" customFormat="1">
+      <c r="A85" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B81" s="50" t="s">
+      <c r="B85" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C81" s="50" t="s">
+      <c r="C85" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D81" s="50" t="s">
+      <c r="D85" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="E81" s="50" t="s">
+      <c r="E85" s="50" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="82" spans="1:17">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F82" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G82" s="30"/>
-      <c r="H82" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I82" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
-      <c r="N82" s="3"/>
-      <c r="P82" s="40"/>
-    </row>
-    <row r="83" spans="1:17" s="43" customFormat="1">
-      <c r="B83" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D83" s="43" t="s">
-        <v>760</v>
-      </c>
-      <c r="E83" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F83" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H83" s="43">
-        <v>0</v>
-      </c>
-      <c r="I83" s="46"/>
-      <c r="J83" s="45">
-        <v>-60</v>
-      </c>
-      <c r="K83" s="45">
-        <v>60</v>
-      </c>
-      <c r="L83" s="45">
-        <v>-1</v>
-      </c>
-      <c r="M83" s="45">
-        <f>(K83-J83)/6</f>
-        <v>20</v>
-      </c>
-      <c r="N83" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="P83" s="47"/>
-      <c r="Q83" s="43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17">
-      <c r="A84" s="30"/>
-      <c r="B84" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84" s="30"/>
-      <c r="D84" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E84" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F84" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G84" s="30"/>
-      <c r="H84" s="30">
-        <v>0</v>
-      </c>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-      <c r="P84" s="40"/>
-    </row>
-    <row r="85" spans="1:17">
-      <c r="A85" s="30"/>
-      <c r="B85" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E85" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F85" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G85" s="30"/>
-      <c r="H85" s="30">
-        <v>0</v>
-      </c>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
-      <c r="L85" s="3"/>
-      <c r="M85" s="3"/>
-      <c r="N85" s="3"/>
-      <c r="P85" s="40"/>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" s="30"/>
@@ -9318,17 +9308,20 @@
       </c>
       <c r="C86" s="30"/>
       <c r="D86" s="30" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F86" s="30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G86" s="30"/>
-      <c r="H86" s="30">
-        <v>0</v>
+      <c r="H86" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I86" s="30" t="s">
+        <v>83</v>
       </c>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
@@ -9337,31 +9330,43 @@
       <c r="N86" s="3"/>
       <c r="P86" s="40"/>
     </row>
-    <row r="87" spans="1:17">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E87" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F87" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G87" s="30"/>
-      <c r="H87" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
-      <c r="M87" s="3"/>
-      <c r="N87" s="3"/>
-      <c r="P87" s="40"/>
+    <row r="87" spans="1:17" s="43" customFormat="1">
+      <c r="B87" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87" s="43" t="s">
+        <v>759</v>
+      </c>
+      <c r="E87" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F87" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H87" s="43">
+        <v>0</v>
+      </c>
+      <c r="I87" s="46"/>
+      <c r="J87" s="45">
+        <v>-60</v>
+      </c>
+      <c r="K87" s="45">
+        <v>60</v>
+      </c>
+      <c r="L87" s="45">
+        <v>-1</v>
+      </c>
+      <c r="M87" s="45">
+        <f>(K87-J87)/6</f>
+        <v>20</v>
+      </c>
+      <c r="N87" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="P87" s="47"/>
+      <c r="Q87" s="43" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="88" spans="1:17">
       <c r="A88" s="30"/>
@@ -9369,18 +9374,18 @@
         <v>21</v>
       </c>
       <c r="C88" s="30"/>
-      <c r="D88" s="30" t="s">
-        <v>55</v>
+      <c r="D88" s="48" t="s">
+        <v>47</v>
       </c>
       <c r="E88" s="30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F88" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G88" s="30"/>
       <c r="H88" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
@@ -9396,10 +9401,10 @@
       </c>
       <c r="C89" s="30"/>
       <c r="D89" s="30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F89" s="30" t="s">
         <v>64</v>
@@ -9422,17 +9427,17 @@
       </c>
       <c r="C90" s="30"/>
       <c r="D90" s="30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F90" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G90" s="30"/>
       <c r="H90" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
@@ -9441,22 +9446,31 @@
       <c r="N90" s="3"/>
       <c r="P90" s="40"/>
     </row>
-    <row r="91" spans="1:17" s="50" customFormat="1">
-      <c r="A91" s="50" t="b">
+    <row r="91" spans="1:17">
+      <c r="A91" s="30"/>
+      <c r="B91" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" s="30"/>
+      <c r="D91" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E91" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F91" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G91" s="30"/>
+      <c r="H91" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="B91" s="50" t="s">
-        <v>327</v>
-      </c>
-      <c r="C91" s="50" t="s">
-        <v>328</v>
-      </c>
-      <c r="D91" s="50" t="s">
-        <v>328</v>
-      </c>
-      <c r="E91" s="50" t="s">
-        <v>68</v>
-      </c>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="P91" s="40"/>
     </row>
     <row r="92" spans="1:17">
       <c r="A92" s="30"/>
@@ -9465,20 +9479,17 @@
       </c>
       <c r="C92" s="30"/>
       <c r="D92" s="30" t="s">
-        <v>373</v>
+        <v>55</v>
       </c>
       <c r="E92" s="30" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F92" s="30" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G92" s="30"/>
-      <c r="H92" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I92" s="30" t="s">
-        <v>83</v>
+      <c r="H92" s="30">
+        <v>15</v>
       </c>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -9487,123 +9498,113 @@
       <c r="N92" s="3"/>
       <c r="P92" s="40"/>
     </row>
-    <row r="93" spans="1:17" s="43" customFormat="1">
-      <c r="B93" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D93" s="43" t="s">
-        <v>778</v>
-      </c>
-      <c r="E93" s="43" t="s">
-        <v>330</v>
-      </c>
-      <c r="F93" s="43" t="s">
+    <row r="93" spans="1:17">
+      <c r="A93" s="30"/>
+      <c r="B93" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E93" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F93" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H93" s="43">
-        <v>0</v>
-      </c>
-      <c r="I93" s="46"/>
-      <c r="J93" s="45">
-        <v>-30</v>
-      </c>
-      <c r="K93" s="45">
-        <v>30</v>
-      </c>
-      <c r="L93" s="45">
-        <v>0</v>
-      </c>
-      <c r="M93" s="45">
-        <f>(K93-J93)/6</f>
-        <v>10</v>
-      </c>
-      <c r="N93" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q93" s="43" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" s="50" customFormat="1">
-      <c r="A94" s="50" t="b">
+      <c r="G93" s="30"/>
+      <c r="H93" s="30">
+        <v>0</v>
+      </c>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="P93" s="40"/>
+    </row>
+    <row r="94" spans="1:17">
+      <c r="A94" s="30"/>
+      <c r="B94" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E94" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F94" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G94" s="30"/>
+      <c r="H94" s="30">
         <v>1</v>
       </c>
-      <c r="B94" s="50" t="s">
-        <v>779</v>
-      </c>
-      <c r="C94" s="50" t="s">
-        <v>780</v>
-      </c>
-      <c r="D94" s="50" t="s">
-        <v>780</v>
-      </c>
-      <c r="E94" s="50" t="s">
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="P94" s="40"/>
+    </row>
+    <row r="95" spans="1:17" s="50" customFormat="1">
+      <c r="A95" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B95" s="50" t="s">
+        <v>327</v>
+      </c>
+      <c r="C95" s="50" t="s">
+        <v>328</v>
+      </c>
+      <c r="D95" s="50" t="s">
+        <v>328</v>
+      </c>
+      <c r="E95" s="50" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="43" customFormat="1">
-      <c r="B95" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D95" s="43" t="s">
-        <v>781</v>
-      </c>
-      <c r="E95" s="43" t="s">
-        <v>258</v>
-      </c>
-      <c r="F95" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H95" s="43">
-        <v>0</v>
-      </c>
-      <c r="I95" s="46"/>
-      <c r="J95" s="45">
-        <v>-50</v>
-      </c>
-      <c r="K95" s="45">
-        <v>100</v>
-      </c>
-      <c r="L95" s="45">
-        <v>0</v>
-      </c>
-      <c r="M95" s="45">
-        <f>(K95-J95)/6</f>
-        <v>25</v>
-      </c>
-      <c r="N95" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q95" s="43" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" s="50" customFormat="1">
-      <c r="A96" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B96" s="50" t="s">
-        <v>782</v>
-      </c>
-      <c r="C96" s="50" t="s">
-        <v>783</v>
-      </c>
-      <c r="D96" s="50" t="s">
-        <v>783</v>
-      </c>
-      <c r="E96" s="50" t="s">
-        <v>68</v>
-      </c>
+    <row r="96" spans="1:17">
+      <c r="A96" s="30"/>
+      <c r="B96" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C96" s="30"/>
+      <c r="D96" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E96" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F96" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G96" s="30"/>
+      <c r="H96" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I96" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="P96" s="40"/>
     </row>
     <row r="97" spans="1:17" s="43" customFormat="1">
       <c r="B97" s="43" t="s">
         <v>22</v>
       </c>
       <c r="D97" s="43" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>258</v>
+        <v>330</v>
       </c>
       <c r="F97" s="43" t="s">
         <v>64</v>
@@ -9613,17 +9614,17 @@
       </c>
       <c r="I97" s="46"/>
       <c r="J97" s="45">
-        <v>-50</v>
+        <v>-30</v>
       </c>
       <c r="K97" s="45">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="L97" s="45">
         <v>0</v>
       </c>
       <c r="M97" s="45">
         <f>(K97-J97)/6</f>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="N97" s="45">
         <v>2.5</v>
@@ -9637,116 +9638,124 @@
         <v>1</v>
       </c>
       <c r="B98" s="50" t="s">
-        <v>285</v>
+        <v>778</v>
       </c>
       <c r="C98" s="50" t="s">
-        <v>286</v>
+        <v>779</v>
       </c>
       <c r="D98" s="50" t="s">
-        <v>286</v>
+        <v>779</v>
       </c>
       <c r="E98" s="50" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="99" spans="1:17" s="30" customFormat="1">
-      <c r="B99" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D99" s="30" t="s">
-        <v>373</v>
-      </c>
-      <c r="E99" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F99" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H99" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I99" s="30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" s="43" customFormat="1">
-      <c r="B100" s="43" t="s">
+    <row r="99" spans="1:17" s="43" customFormat="1">
+      <c r="B99" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D100" s="43" t="s">
-        <v>785</v>
-      </c>
-      <c r="E100" s="43" t="s">
-        <v>288</v>
-      </c>
-      <c r="F100" s="43" t="s">
+      <c r="D99" s="43" t="s">
+        <v>780</v>
+      </c>
+      <c r="E99" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="F99" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G100" s="43" t="s">
-        <v>786</v>
-      </c>
-      <c r="H100" s="43">
-        <v>0</v>
-      </c>
-      <c r="I100" s="46"/>
-      <c r="J100" s="45">
-        <v>-40</v>
-      </c>
-      <c r="K100" s="45">
-        <v>80</v>
-      </c>
-      <c r="L100" s="45">
-        <v>-1</v>
-      </c>
-      <c r="M100" s="45">
-        <f>(K100-J100)/6</f>
-        <v>20</v>
-      </c>
-      <c r="N100" s="45">
+      <c r="H99" s="43">
+        <v>0</v>
+      </c>
+      <c r="I99" s="46"/>
+      <c r="J99" s="45">
+        <v>-50</v>
+      </c>
+      <c r="K99" s="45">
+        <v>100</v>
+      </c>
+      <c r="L99" s="45">
+        <v>0</v>
+      </c>
+      <c r="M99" s="45">
+        <f>(K99-J99)/6</f>
+        <v>25</v>
+      </c>
+      <c r="N99" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q100" s="43" t="s">
+      <c r="Q99" s="43" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="101" spans="1:17" s="30" customFormat="1">
-      <c r="B101" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D101" s="30" t="s">
-        <v>787</v>
-      </c>
-      <c r="E101" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F101" s="30" t="s">
+    <row r="100" spans="1:17" s="50" customFormat="1">
+      <c r="A100" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B100" s="50" t="s">
+        <v>781</v>
+      </c>
+      <c r="C100" s="50" t="s">
+        <v>782</v>
+      </c>
+      <c r="D100" s="50" t="s">
+        <v>782</v>
+      </c>
+      <c r="E100" s="50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" s="43" customFormat="1">
+      <c r="B101" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" s="43" t="s">
+        <v>783</v>
+      </c>
+      <c r="E101" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="F101" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G101" s="30" t="s">
-        <v>786</v>
-      </c>
-      <c r="H101" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" s="30" customFormat="1">
-      <c r="B102" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D102" s="30" t="s">
-        <v>788</v>
-      </c>
-      <c r="E102" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F102" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G102" s="30" t="s">
-        <v>786</v>
-      </c>
-      <c r="H102" s="30">
-        <v>0</v>
+      <c r="H101" s="43">
+        <v>0</v>
+      </c>
+      <c r="I101" s="46"/>
+      <c r="J101" s="45">
+        <v>-50</v>
+      </c>
+      <c r="K101" s="45">
+        <v>100</v>
+      </c>
+      <c r="L101" s="45">
+        <v>0</v>
+      </c>
+      <c r="M101" s="45">
+        <f>(K101-J101)/6</f>
+        <v>25</v>
+      </c>
+      <c r="N101" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q101" s="43" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" s="50" customFormat="1">
+      <c r="A102" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B102" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="C102" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="D102" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="E102" s="50" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="30" customFormat="1">
@@ -9754,36 +9763,59 @@
         <v>21</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>789</v>
+        <v>373</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F103" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G103" s="30" t="s">
-        <v>790</v>
-      </c>
-      <c r="H103" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" s="30" customFormat="1">
-      <c r="B104" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D104" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="E104" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F104" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H104" s="30" t="b">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="H103" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I103" s="30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" s="43" customFormat="1">
+      <c r="B104" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" s="43" t="s">
+        <v>784</v>
+      </c>
+      <c r="E104" s="43" t="s">
+        <v>288</v>
+      </c>
+      <c r="F104" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G104" s="43" t="s">
+        <v>785</v>
+      </c>
+      <c r="H104" s="43">
+        <v>0</v>
+      </c>
+      <c r="I104" s="46"/>
+      <c r="J104" s="45">
+        <v>-40</v>
+      </c>
+      <c r="K104" s="45">
+        <v>80</v>
+      </c>
+      <c r="L104" s="45">
+        <v>-1</v>
+      </c>
+      <c r="M104" s="45">
+        <f>(K104-J104)/6</f>
+        <v>20</v>
+      </c>
+      <c r="N104" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q104" s="43" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="30" customFormat="1">
@@ -9791,19 +9823,19 @@
         <v>21</v>
       </c>
       <c r="D105" s="30" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F105" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G105" s="30" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="H105" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="30" customFormat="1">
@@ -9811,16 +9843,16 @@
         <v>21</v>
       </c>
       <c r="D106" s="30" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F106" s="30" t="s">
         <v>64</v>
       </c>
       <c r="G106" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H106" s="30">
         <v>0</v>
@@ -9831,207 +9863,268 @@
         <v>21</v>
       </c>
       <c r="D107" s="30" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="E107" s="30" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F107" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G107" s="30" t="s">
+        <v>789</v>
+      </c>
+      <c r="H107" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" s="30" customFormat="1">
+      <c r="B108" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="30" t="s">
         <v>790</v>
       </c>
-      <c r="H107" s="30">
+      <c r="E108" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F108" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H108" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" s="30" customFormat="1">
+      <c r="B109" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" s="30" t="s">
+        <v>791</v>
+      </c>
+      <c r="E109" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F109" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G109" s="30" t="s">
+        <v>789</v>
+      </c>
+      <c r="H109" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" s="30" customFormat="1">
+      <c r="B110" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="E110" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F110" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G110" s="30" t="s">
+        <v>785</v>
+      </c>
+      <c r="H110" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" s="30" customFormat="1">
+      <c r="B111" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" s="30" t="s">
+        <v>793</v>
+      </c>
+      <c r="E111" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G111" s="30" t="s">
+        <v>789</v>
+      </c>
+      <c r="H111" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:17" s="38" customFormat="1">
-      <c r="A108" s="38" t="b">
+    <row r="112" spans="1:17" s="38" customFormat="1">
+      <c r="A112" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B108" s="38" t="s">
+      <c r="B112" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="38" t="s">
+      <c r="C112" s="38" t="s">
+        <v>802</v>
+      </c>
+      <c r="D112" s="38" t="s">
+        <v>802</v>
+      </c>
+      <c r="E112" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G112" s="39"/>
+      <c r="H112" s="39"/>
+    </row>
+    <row r="113" spans="2:17" s="43" customFormat="1">
+      <c r="B113" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D113" s="43" t="s">
         <v>803</v>
       </c>
-      <c r="D108" s="38" t="s">
-        <v>803</v>
-      </c>
-      <c r="E108" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G108" s="39"/>
-      <c r="H108" s="39"/>
-    </row>
-    <row r="109" spans="1:17" s="43" customFormat="1">
-      <c r="B109" s="43" t="s">
+      <c r="E113" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="F113" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G113" s="43" t="s">
+        <v>804</v>
+      </c>
+      <c r="H113" s="43">
+        <v>1</v>
+      </c>
+      <c r="I113" s="46"/>
+      <c r="J113" s="45">
+        <v>-2</v>
+      </c>
+      <c r="K113" s="45">
+        <v>2</v>
+      </c>
+      <c r="L113" s="45">
+        <v>0</v>
+      </c>
+      <c r="M113" s="45">
+        <f>(K113-J113)/6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N113" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q113" s="43" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="114" spans="2:17" s="43" customFormat="1">
+      <c r="B114" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D109" s="43" t="s">
+      <c r="D114" s="43" t="s">
+        <v>805</v>
+      </c>
+      <c r="E114" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="F114" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G114" s="43" t="s">
         <v>804</v>
       </c>
-      <c r="E109" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="F109" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G109" s="43" t="s">
-        <v>805</v>
-      </c>
-      <c r="H109" s="43">
+      <c r="H114" s="43">
+        <v>-1</v>
+      </c>
+      <c r="I114" s="46"/>
+      <c r="J114" s="45">
+        <v>-2</v>
+      </c>
+      <c r="K114" s="45">
+        <v>2</v>
+      </c>
+      <c r="L114" s="45">
+        <v>0</v>
+      </c>
+      <c r="M114" s="45">
+        <f>(K114-J114)/6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N114" s="45">
         <v>1</v>
       </c>
-      <c r="I109" s="46"/>
-      <c r="J109" s="45">
-        <v>-2</v>
-      </c>
-      <c r="K109" s="45">
-        <v>2</v>
-      </c>
-      <c r="L109" s="45">
-        <v>0</v>
-      </c>
-      <c r="M109" s="45">
-        <f>(K109-J109)/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="N109" s="45">
-        <v>1</v>
-      </c>
-      <c r="Q109" s="43" t="s">
+      <c r="Q114" s="43" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="110" spans="1:17" s="43" customFormat="1">
-      <c r="B110" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D110" s="43" t="s">
+    <row r="115" spans="2:17">
+      <c r="B115" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115" s="31" t="s">
         <v>806</v>
       </c>
-      <c r="E110" s="43" t="s">
-        <v>192</v>
-      </c>
-      <c r="F110" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G110" s="43" t="s">
-        <v>805</v>
-      </c>
-      <c r="H110" s="43">
-        <v>-1</v>
-      </c>
-      <c r="I110" s="46"/>
-      <c r="J110" s="45">
-        <v>-2</v>
-      </c>
-      <c r="K110" s="45">
-        <v>2</v>
-      </c>
-      <c r="L110" s="45">
-        <v>0</v>
-      </c>
-      <c r="M110" s="45">
-        <f>(K110-J110)/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="N110" s="45">
-        <v>1</v>
-      </c>
-      <c r="Q110" s="43" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="111" spans="1:17">
-      <c r="B111" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D111" s="31" t="s">
-        <v>807</v>
-      </c>
-      <c r="E111" s="31" t="s">
+      <c r="E115" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="F111" s="31" t="s">
+      <c r="F115" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="H111" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J111" s="3"/>
-      <c r="K111" s="3"/>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
-    </row>
-    <row r="112" spans="1:17">
-      <c r="H112" s="31"/>
-      <c r="I112" s="31"/>
-    </row>
-    <row r="113" spans="8:9">
-      <c r="H113" s="31"/>
-      <c r="I113" s="31"/>
-    </row>
-    <row r="114" spans="8:9">
-      <c r="H114" s="31"/>
-      <c r="I114" s="31"/>
-    </row>
-    <row r="115" spans="8:9">
-      <c r="H115" s="31"/>
-      <c r="I115" s="31"/>
-    </row>
-    <row r="116" spans="8:9">
+      <c r="H115" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="3"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+    </row>
+    <row r="116" spans="2:17">
       <c r="H116" s="31"/>
       <c r="I116" s="31"/>
     </row>
-    <row r="117" spans="8:9">
+    <row r="117" spans="2:17">
       <c r="H117" s="31"/>
       <c r="I117" s="31"/>
     </row>
-    <row r="118" spans="8:9">
+    <row r="118" spans="2:17">
       <c r="H118" s="31"/>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="8:9">
+    <row r="119" spans="2:17">
       <c r="H119" s="31"/>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="8:9">
+    <row r="120" spans="2:17">
       <c r="H120" s="31"/>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="8:9">
+    <row r="121" spans="2:17">
       <c r="H121" s="31"/>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="8:9">
+    <row r="122" spans="2:17">
       <c r="H122" s="31"/>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="8:9">
+    <row r="123" spans="2:17">
       <c r="H123" s="31"/>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="8:9">
+    <row r="124" spans="2:17">
       <c r="H124" s="31"/>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="8:9">
+    <row r="125" spans="2:17">
       <c r="H125" s="31"/>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="8:9">
+    <row r="126" spans="2:17">
       <c r="H126" s="31"/>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="8:9">
+    <row r="127" spans="2:17">
       <c r="H127" s="31"/>
       <c r="I127" s="31"/>
     </row>
-    <row r="128" spans="8:9">
+    <row r="128" spans="2:17">
       <c r="H128" s="31"/>
       <c r="I128" s="31"/>
     </row>
@@ -10431,8 +10524,24 @@
       <c r="H227" s="31"/>
       <c r="I227" s="31"/>
     </row>
+    <row r="228" spans="8:9">
+      <c r="H228" s="31"/>
+      <c r="I228" s="31"/>
+    </row>
+    <row r="229" spans="8:9">
+      <c r="H229" s="31"/>
+      <c r="I229" s="31"/>
+    </row>
+    <row r="230" spans="8:9">
+      <c r="H230" s="31"/>
+      <c r="I230" s="31"/>
+    </row>
+    <row r="231" spans="8:9">
+      <c r="H231" s="31"/>
+      <c r="I231" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z154"/>
+  <autoFilter ref="A2:Z158"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>
@@ -10677,7 +10786,7 @@
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>707</v>
@@ -10705,7 +10814,7 @@
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>709</v>
@@ -10729,14 +10838,14 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="30" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>64</v>
@@ -10756,14 +10865,14 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="30" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>64</v>
@@ -10783,14 +10892,14 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="30" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>64</v>
@@ -10810,14 +10919,14 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="30" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>64</v>

</xml_diff>